<commit_message>
added one more field director as an example
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/WD/Movies.External/miniDV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EE05A79-F0FD-B943-A6F7-0BC240BE45BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09472A93-EC0F-3E4F-B108-8FBDEA20BB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="6900" windowWidth="26840" windowHeight="15940" xr2:uid="{FFFC5904-6A26-034F-8A25-8F3A42E4F918}"/>
+    <workbookView xWindow="5600" yWindow="6360" windowWidth="45540" windowHeight="15940" xr2:uid="{FFFC5904-6A26-034F-8A25-8F3A42E4F918}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>xml filename</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Family activities Video Recordings throughout the years.</t>
   </si>
   <si>
-    <t>2023-05-01_Camera_001_x264_720x576/2023-05-01_Camera_001_x264_720x576.nfo</t>
-  </si>
-  <si>
     <t>2001-05-01 Camera 001</t>
   </si>
   <si>
@@ -72,6 +69,18 @@
   </si>
   <si>
     <t>Camera</t>
+  </si>
+  <si>
+    <t>example/example.nfo</t>
+  </si>
+  <si>
+    <t>movie/director:string</t>
+  </si>
+  <si>
+    <t>Spielberg</t>
+  </si>
+  <si>
+    <t>2023-05-01</t>
   </si>
 </sst>
 </file>
@@ -109,7 +118,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642D6711-417A-0142-9A9E-E4BD0272BB27}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,7 +469,7 @@
     <col min="7" max="7" width="46.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,28 +491,34 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="1">
-        <v>45047</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>